<commit_message>
ajuste de gastos nov
</commit_message>
<xml_diff>
--- a/Balance_2024.xlsx
+++ b/Balance_2024.xlsx
@@ -891,7 +891,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1103,6 +1103,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -6948,8 +6951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -7515,7 +7518,7 @@
         <f>IF(F32 &lt; J32,"SALDO A FAVOR",IF(F32&gt;J32,"SALDO PENDIENTE","IGUAL"))</f>
         <v>SALDO A FAVOR</v>
       </c>
-      <c r="F33" s="16">
+      <c r="F33" s="71">
         <f>+J32-F32</f>
         <v>3405511</v>
       </c>
@@ -7545,6 +7548,9 @@
       <c r="H36" s="41"/>
     </row>
     <row r="37" spans="5:8">
+      <c r="F37">
+        <v>700000</v>
+      </c>
       <c r="G37" s="40" t="s">
         <v>137</v>
       </c>

</xml_diff>